<commit_message>
final update before advisor review
</commit_message>
<xml_diff>
--- a/data/variablebook.xlsx
+++ b/data/variablebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\TPESS-GGM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\TPESS-Network-S1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD8EB68-B097-4D09-9178-D96148D48646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7020D3C2-5C69-40DC-9CB5-FEB0B8F3A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4718,9 +4718,6 @@
     <t>Anxious feelings</t>
   </si>
   <si>
-    <t>Control of anxeity</t>
-  </si>
-  <si>
     <t>Difficulty relaxing</t>
   </si>
   <si>
@@ -5037,6 +5034,9 @@
   </si>
   <si>
     <t>Suicidality</t>
+  </si>
+  <si>
+    <t>Control of anxiety</t>
   </si>
 </sst>
 </file>
@@ -5399,8 +5399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5418,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -5430,7 +5430,7 @@
         <v>1210</v>
       </c>
       <c r="F1" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5494,7 +5494,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1308</v>
@@ -5514,7 +5514,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -5534,7 +5534,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -5554,7 +5554,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
@@ -5574,7 +5574,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -5594,7 +5594,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -5614,7 +5614,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -5634,7 +5634,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -5654,7 +5654,7 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>29</v>
@@ -5674,7 +5674,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -5694,7 +5694,7 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
@@ -5714,7 +5714,7 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>35</v>
@@ -5734,7 +5734,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>37</v>
@@ -5754,7 +5754,7 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>39</v>
@@ -5774,7 +5774,7 @@
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>41</v>
@@ -5794,7 +5794,7 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>43</v>
@@ -5814,7 +5814,7 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>45</v>
@@ -5834,7 +5834,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>47</v>
@@ -5854,7 +5854,7 @@
         <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>49</v>
@@ -5874,7 +5874,7 @@
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>51</v>
@@ -5894,7 +5894,7 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
@@ -5914,7 +5914,7 @@
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>55</v>
@@ -5926,7 +5926,7 @@
         <v>1212</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>1466</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5934,7 +5934,7 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>57</v>
@@ -5946,7 +5946,7 @@
         <v>1212</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5954,7 +5954,7 @@
         <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>59</v>
@@ -5966,7 +5966,7 @@
         <v>1212</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5974,7 +5974,7 @@
         <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>61</v>
@@ -5986,7 +5986,7 @@
         <v>1212</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5994,7 +5994,7 @@
         <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>63</v>
@@ -6006,7 +6006,7 @@
         <v>1212</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6014,7 +6014,7 @@
         <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>65</v>
@@ -6026,7 +6026,7 @@
         <v>1212</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6034,7 +6034,7 @@
         <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>67</v>
@@ -6046,7 +6046,7 @@
         <v>1213</v>
       </c>
       <c r="F36" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6054,7 +6054,7 @@
         <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>69</v>
@@ -6074,7 +6074,7 @@
         <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>71</v>
@@ -6094,7 +6094,7 @@
         <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>73</v>
@@ -6114,7 +6114,7 @@
         <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>75</v>
@@ -6134,7 +6134,7 @@
         <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>77</v>
@@ -6146,7 +6146,7 @@
         <v>1213</v>
       </c>
       <c r="F41" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6154,7 +6154,7 @@
         <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>79</v>
@@ -6174,7 +6174,7 @@
         <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>81</v>
@@ -6194,7 +6194,7 @@
         <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>83</v>
@@ -6206,7 +6206,7 @@
         <v>1213</v>
       </c>
       <c r="F44" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -6214,7 +6214,7 @@
         <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C45" t="s">
         <v>1399</v>
@@ -6226,7 +6226,7 @@
         <v>1214</v>
       </c>
       <c r="F45" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -6234,7 +6234,7 @@
         <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="C46" t="s">
         <v>1400</v>
@@ -6246,7 +6246,7 @@
         <v>1214</v>
       </c>
       <c r="F46" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -6254,7 +6254,7 @@
         <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="C47" t="s">
         <v>1401</v>
@@ -6266,7 +6266,7 @@
         <v>1214</v>
       </c>
       <c r="F47" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -6274,7 +6274,7 @@
         <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C48" t="s">
         <v>1408</v>
@@ -6286,7 +6286,7 @@
         <v>1214</v>
       </c>
       <c r="F48" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -6294,7 +6294,7 @@
         <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="C49" t="s">
         <v>1402</v>
@@ -6306,7 +6306,7 @@
         <v>1214</v>
       </c>
       <c r="F49" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -6314,7 +6314,7 @@
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="C50" t="s">
         <v>1403</v>
@@ -6326,7 +6326,7 @@
         <v>1214</v>
       </c>
       <c r="F50" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -6334,7 +6334,7 @@
         <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C51" t="s">
         <v>1404</v>
@@ -6346,7 +6346,7 @@
         <v>1214</v>
       </c>
       <c r="F51" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -6354,7 +6354,7 @@
         <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="C52" t="s">
         <v>1405</v>
@@ -6366,7 +6366,7 @@
         <v>1214</v>
       </c>
       <c r="F52" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -6374,7 +6374,7 @@
         <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="C53" t="s">
         <v>1406</v>
@@ -6386,7 +6386,7 @@
         <v>1214</v>
       </c>
       <c r="F53" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -6394,7 +6394,7 @@
         <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C54" t="s">
         <v>1407</v>
@@ -6406,7 +6406,7 @@
         <v>1214</v>
       </c>
       <c r="F54" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -6414,7 +6414,7 @@
         <v>94</v>
       </c>
       <c r="B55" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="C55" t="s">
         <v>1419</v>
@@ -6423,10 +6423,10 @@
         <v>1429</v>
       </c>
       <c r="E55" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F55" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -6434,7 +6434,7 @@
         <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C56" t="s">
         <v>1420</v>
@@ -6443,10 +6443,10 @@
         <v>1430</v>
       </c>
       <c r="E56" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F56" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -6454,7 +6454,7 @@
         <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="C57" t="s">
         <v>1421</v>
@@ -6463,10 +6463,10 @@
         <v>1431</v>
       </c>
       <c r="E57" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F57" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -6474,7 +6474,7 @@
         <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="C58" t="s">
         <v>1422</v>
@@ -6483,10 +6483,10 @@
         <v>1432</v>
       </c>
       <c r="E58" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F58" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -6494,7 +6494,7 @@
         <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="C59" t="s">
         <v>1423</v>
@@ -6503,10 +6503,10 @@
         <v>1433</v>
       </c>
       <c r="E59" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F59" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
         <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="C60" t="s">
         <v>1424</v>
@@ -6523,10 +6523,10 @@
         <v>1434</v>
       </c>
       <c r="E60" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F60" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>100</v>
       </c>
       <c r="B61" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="C61" t="s">
         <v>1425</v>
@@ -6543,10 +6543,10 @@
         <v>1435</v>
       </c>
       <c r="E61" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F61" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -6554,7 +6554,7 @@
         <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C62" t="s">
         <v>1426</v>
@@ -6563,10 +6563,10 @@
         <v>1436</v>
       </c>
       <c r="E62" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F62" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -6574,7 +6574,7 @@
         <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="C63" t="s">
         <v>1427</v>
@@ -6583,10 +6583,10 @@
         <v>1437</v>
       </c>
       <c r="E63" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F63" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -6594,7 +6594,7 @@
         <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="C64" t="s">
         <v>1428</v>
@@ -6603,10 +6603,10 @@
         <v>1438</v>
       </c>
       <c r="E64" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F64" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -11489,58 +11489,58 @@
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B509" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D509" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="F509" s="1" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B510" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="D510" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="F510" s="1" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B511" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D511" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="F511" s="1" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B512" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D512" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="F512" s="1" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
@@ -11595,7 +11595,7 @@
         <v>3</v>
       </c>
       <c r="D517" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
@@ -13503,16 +13503,16 @@
         <v>1157</v>
       </c>
       <c r="B679" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D679" s="1" t="s">
         <v>1339</v>
       </c>
       <c r="E679" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="F679" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="680" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changing node label + updating cfmnetwork code
</commit_message>
<xml_diff>
--- a/data/variablebook.xlsx
+++ b/data/variablebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\TPESS-Network-S1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7020D3C2-5C69-40DC-9CB5-FEB0B8F3A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D24EBF-E8E1-43AC-A8F9-08AEE4C0D81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4937,9 +4937,6 @@
     <t>S10</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>TPESS mean score</t>
   </si>
   <si>
@@ -5037,6 +5034,9 @@
   </si>
   <si>
     <t>Control of anxiety</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -5399,8 +5399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A668" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B679" sqref="B679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5494,7 +5494,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1308</v>
@@ -5514,7 +5514,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -5534,7 +5534,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -5554,7 +5554,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
@@ -5574,7 +5574,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -5594,7 +5594,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -5614,7 +5614,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -5634,7 +5634,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -5654,7 +5654,7 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>29</v>
@@ -5674,7 +5674,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>31</v>
@@ -5694,7 +5694,7 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
@@ -5714,7 +5714,7 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>35</v>
@@ -5734,7 +5734,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>37</v>
@@ -5754,7 +5754,7 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>39</v>
@@ -5774,7 +5774,7 @@
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>41</v>
@@ -5794,7 +5794,7 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>43</v>
@@ -5814,7 +5814,7 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>45</v>
@@ -5834,7 +5834,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>47</v>
@@ -5854,7 +5854,7 @@
         <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>49</v>
@@ -5874,7 +5874,7 @@
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>51</v>
@@ -5926,7 +5926,7 @@
         <v>1212</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6046,7 +6046,7 @@
         <v>1213</v>
       </c>
       <c r="F36" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6146,7 +6146,7 @@
         <v>1213</v>
       </c>
       <c r="F41" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6206,7 +6206,7 @@
         <v>1213</v>
       </c>
       <c r="F44" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -11492,13 +11492,13 @@
         <v>1476</v>
       </c>
       <c r="B509" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D509" t="s">
         <v>1475</v>
       </c>
       <c r="F509" s="1" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
@@ -11506,13 +11506,13 @@
         <v>1477</v>
       </c>
       <c r="B510" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D510" t="s">
         <v>1474</v>
       </c>
       <c r="F510" s="1" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
@@ -11520,13 +11520,13 @@
         <v>1471</v>
       </c>
       <c r="B511" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="D511" t="s">
         <v>1473</v>
       </c>
       <c r="F511" s="1" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
@@ -11534,13 +11534,13 @@
         <v>1478</v>
       </c>
       <c r="B512" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D512" t="s">
         <v>1472</v>
       </c>
       <c r="F512" s="1" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
@@ -13503,16 +13503,16 @@
         <v>1157</v>
       </c>
       <c r="B679" t="s">
-        <v>1539</v>
+        <v>1572</v>
       </c>
       <c r="D679" s="1" t="s">
         <v>1339</v>
       </c>
       <c r="E679" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="F679" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="680" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update for paper revision
</commit_message>
<xml_diff>
--- a/data/variablebook.xlsx
+++ b/data/variablebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\TPESS-Network-S1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leong\OneDrive\Documents\Github\TPESS-Network-S1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D24EBF-E8E1-43AC-A8F9-08AEE4C0D81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C693561-A92D-4C85-AE10-4511B1007EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1593">
   <si>
     <t>variablename</t>
   </si>
@@ -5037,6 +5037,66 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>Repetitive Negative Thinking subscale</t>
+  </si>
+  <si>
+    <t>Intolerance of Uncertainty subscale</t>
+  </si>
+  <si>
+    <t>Affect Sensitivity subscale</t>
+  </si>
+  <si>
+    <t>Affect Intolerance subscale</t>
+  </si>
+  <si>
+    <t>Reactivity to Diffused Threat subscale</t>
+  </si>
+  <si>
+    <t>Cognitive Avoidance subscale</t>
+  </si>
+  <si>
+    <t>Negative Self-Regard subscale</t>
+  </si>
+  <si>
+    <t>Need for Social Approval subscale</t>
+  </si>
+  <si>
+    <t>Percieved and Expected Loss subscale</t>
+  </si>
+  <si>
+    <t>(Percieved) Uncontrollability to External Events subscale</t>
   </si>
 </sst>
 </file>
@@ -5399,8 +5459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A668" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B679" sqref="B679"/>
+    <sheetView tabSelected="1" topLeftCell="C653" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F683" sqref="F683:F684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13332,6 +13392,9 @@
       <c r="A669" t="s">
         <v>1147</v>
       </c>
+      <c r="B669" t="s">
+        <v>1573</v>
+      </c>
       <c r="C669" s="1" t="s">
         <v>3</v>
       </c>
@@ -13341,14 +13404,17 @@
       <c r="E669" t="s">
         <v>1240</v>
       </c>
-      <c r="F669" t="s">
-        <v>1230</v>
+      <c r="F669" s="1" t="s">
+        <v>1583</v>
       </c>
     </row>
     <row r="670" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
         <v>1148</v>
       </c>
+      <c r="B670" t="s">
+        <v>1574</v>
+      </c>
       <c r="C670" s="1" t="s">
         <v>3</v>
       </c>
@@ -13358,14 +13424,17 @@
       <c r="E670" t="s">
         <v>1241</v>
       </c>
-      <c r="F670" t="s">
-        <v>1231</v>
+      <c r="F670" s="1" t="s">
+        <v>1584</v>
       </c>
     </row>
     <row r="671" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
         <v>1149</v>
       </c>
+      <c r="B671" t="s">
+        <v>1575</v>
+      </c>
       <c r="C671" s="1" t="s">
         <v>3</v>
       </c>
@@ -13375,14 +13444,17 @@
       <c r="E671" t="s">
         <v>1242</v>
       </c>
-      <c r="F671" t="s">
-        <v>1232</v>
+      <c r="F671" s="1" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
         <v>1150</v>
       </c>
+      <c r="B672" t="s">
+        <v>1576</v>
+      </c>
       <c r="C672" s="1" t="s">
         <v>3</v>
       </c>
@@ -13392,14 +13464,17 @@
       <c r="E672" t="s">
         <v>1243</v>
       </c>
-      <c r="F672" t="s">
-        <v>1233</v>
+      <c r="F672" s="1" t="s">
+        <v>1586</v>
       </c>
     </row>
     <row r="673" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
         <v>1151</v>
       </c>
+      <c r="B673" t="s">
+        <v>1577</v>
+      </c>
       <c r="C673" s="1" t="s">
         <v>3</v>
       </c>
@@ -13409,14 +13484,17 @@
       <c r="E673" t="s">
         <v>1244</v>
       </c>
-      <c r="F673" t="s">
-        <v>1234</v>
+      <c r="F673" s="1" t="s">
+        <v>1587</v>
       </c>
     </row>
     <row r="674" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
         <v>1152</v>
       </c>
+      <c r="B674" t="s">
+        <v>1578</v>
+      </c>
       <c r="C674" s="1" t="s">
         <v>3</v>
       </c>
@@ -13426,14 +13504,17 @@
       <c r="E674" t="s">
         <v>1245</v>
       </c>
-      <c r="F674" t="s">
-        <v>1235</v>
+      <c r="F674" s="1" t="s">
+        <v>1588</v>
       </c>
     </row>
     <row r="675" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
         <v>1153</v>
       </c>
+      <c r="B675" t="s">
+        <v>1579</v>
+      </c>
       <c r="C675" s="1" t="s">
         <v>3</v>
       </c>
@@ -13443,14 +13524,17 @@
       <c r="E675" t="s">
         <v>1246</v>
       </c>
-      <c r="F675" t="s">
-        <v>1236</v>
+      <c r="F675" s="1" t="s">
+        <v>1589</v>
       </c>
     </row>
     <row r="676" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
         <v>1154</v>
       </c>
+      <c r="B676" t="s">
+        <v>1580</v>
+      </c>
       <c r="C676" s="1" t="s">
         <v>3</v>
       </c>
@@ -13460,14 +13544,17 @@
       <c r="E676" t="s">
         <v>1247</v>
       </c>
-      <c r="F676" t="s">
-        <v>1237</v>
+      <c r="F676" s="1" t="s">
+        <v>1590</v>
       </c>
     </row>
     <row r="677" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
         <v>1155</v>
       </c>
+      <c r="B677" t="s">
+        <v>1581</v>
+      </c>
       <c r="C677" s="1" t="s">
         <v>3</v>
       </c>
@@ -13477,14 +13564,17 @@
       <c r="E677" t="s">
         <v>1248</v>
       </c>
-      <c r="F677" t="s">
-        <v>1238</v>
+      <c r="F677" s="1" t="s">
+        <v>1591</v>
       </c>
     </row>
     <row r="678" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
         <v>1156</v>
       </c>
+      <c r="B678" t="s">
+        <v>1582</v>
+      </c>
       <c r="C678" s="1" t="s">
         <v>3</v>
       </c>
@@ -13494,8 +13584,8 @@
       <c r="E678" t="s">
         <v>1249</v>
       </c>
-      <c r="F678" t="s">
-        <v>1239</v>
+      <c r="F678" s="1" t="s">
+        <v>1592</v>
       </c>
     </row>
     <row r="679" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>